<commit_message>
1.0.5 - simplified Agent inputs: trimmed details table, added Page to document text.
</commit_message>
<xml_diff>
--- a/Data/Input/ResultsTemplate.xlsx
+++ b/Data/Input/ResultsTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/richard_king_uipath_com/Documents/Documents/Diamondback/OpenTicket_Audit/Data/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="135" documentId="11_F25DC773A252ABDACC1048D9895C53825ADE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3027FB8F-FD5E-46DA-A0BE-23ABB92DFE0B}"/>
+  <xr:revisionPtr revIDLastSave="138" documentId="11_F25DC773A252ABDACC1048D9895C53825ADE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B05A48E1-E81C-440A-9B37-8F28539FB636}"/>
   <bookViews>
-    <workbookView xWindow="-29100" yWindow="-7590" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-300" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -117,16 +117,16 @@
     <t>Audit failed reasons: Currency not USD;Service Date mismatch;Total Amount mismatch;Fluid Hauled mismatch;Volume mismatch; Price Book missing;</t>
   </si>
   <si>
-    <t>Rate mismatch and Total Amount mismatch</t>
-  </si>
-  <si>
-    <t>Audit failed reasons: Ticket Number mismatch;Price Book missing;</t>
-  </si>
-  <si>
     <t>Audit failed reasons: Ticket image missing;</t>
   </si>
   <si>
-    <t>Audit failed reasons: ; Price Book missing;Disposal Ticket mismatch</t>
+    <t>Audit failed reasons: Total Amount mismatch;Rate mismatch; Price Book missing;</t>
+  </si>
+  <si>
+    <t>Audit failed reasons: Ticket Number mismatch; Price Book missing;</t>
+  </si>
+  <si>
+    <t>Audit failed reasons: Disposal Ticket mismatch; Price Book missing;</t>
   </si>
 </sst>
 </file>
@@ -538,9 +538,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1788,8 +1788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98FA38FB-2EF5-4767-8D99-2395F6EBE707}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1899,7 +1899,7 @@
         <v>14</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="54" customHeight="1" x14ac:dyDescent="0.3">
@@ -1939,7 +1939,7 @@
         <v>212117</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="54" customHeight="1" x14ac:dyDescent="0.3">
@@ -1947,7 +1947,7 @@
         <v>217299</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>